<commit_message>
Motion Lidt forklaring til Move funktionen Semikolon i RobotController (skønhedsfejl)
</commit_message>
<xml_diff>
--- a/Software/Formelberegning.xlsx
+++ b/Software/Formelberegning.xlsx
@@ -323,11 +323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="387708528"/>
-        <c:axId val="387712448"/>
+        <c:axId val="196059880"/>
+        <c:axId val="196062232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="387708528"/>
+        <c:axId val="196059880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,6 +347,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance [mm]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -384,12 +440,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387712448"/>
+        <c:crossAx val="196062232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="387712448"/>
+        <c:axId val="196062232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -409,6 +465,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -446,7 +558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387708528"/>
+        <c:crossAx val="196059880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -767,11 +879,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="387707352"/>
-        <c:axId val="387709312"/>
+        <c:axId val="196063408"/>
+        <c:axId val="196060272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="387707352"/>
+        <c:axId val="196063408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,6 +903,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Angle</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>deg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -828,12 +1004,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387709312"/>
+        <c:crossAx val="196060272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="387709312"/>
+        <c:axId val="196060272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,6 +1029,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -890,7 +1122,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387707352"/>
+        <c:crossAx val="196063408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1181,11 +1413,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188396248"/>
-        <c:axId val="188398992"/>
+        <c:axId val="196063800"/>
+        <c:axId val="196057136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188396248"/>
+        <c:axId val="196063800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,6 +1437,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Angle [deg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1242,12 +1530,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188398992"/>
+        <c:crossAx val="196057136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188398992"/>
+        <c:axId val="196057136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1267,6 +1555,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1304,7 +1648,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188396248"/>
+        <c:crossAx val="196063800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3385,8 +3729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>